<commit_message>
chanche xml and exel file
</commit_message>
<xml_diff>
--- a/firstWpf/doc.xlsx
+++ b/firstWpf/doc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="188">
   <si>
     <t>Кустовое  основание</t>
   </si>
@@ -212,7 +212,7 @@
     <t>Разработка грунта в отвал экскаваторами "драглайн" или "обратная лопата" с ковшом вместимостью: 0,65 (0,5-1) м3, группа грунтов 1</t>
   </si>
   <si>
-    <t>0,0492</t>
+    <t>0,049</t>
   </si>
   <si>
     <t>18,05</t>
@@ -281,7 +281,7 @@
     <t>т</t>
   </si>
   <si>
-    <t>0,3781470</t>
+    <t>0,378</t>
   </si>
   <si>
     <t>ТЕР01-01-034-02</t>
@@ -323,10 +323,10 @@
     <t>12,18</t>
   </si>
   <si>
-    <t>0,018230500000000000000000000</t>
-  </si>
-  <si>
-    <t>0,0607683333333333333333333333</t>
+    <t>0,018</t>
+  </si>
+  <si>
+    <t>0,061</t>
   </si>
   <si>
     <t>ТСЦпг310-3016-1</t>
@@ -341,7 +341,7 @@
     <t>Разработка грунта с перемещением грунта до 10 м бульдозерами мощностью: 340 кВт (450 л.с.), группа грунтов 1</t>
   </si>
   <si>
-    <t>0,1215366666666666666666666667</t>
+    <t>0,122</t>
   </si>
   <si>
     <t>1,76</t>
@@ -443,7 +443,7 @@
     <t>Природоохранные   мероприятия</t>
   </si>
   <si>
-    <t>0,0777</t>
+    <t>0,078</t>
   </si>
   <si>
     <t>0,259</t>
@@ -464,19 +464,13 @@
     <t>0,2</t>
   </si>
   <si>
-    <t>0,0486024</t>
-  </si>
-  <si>
-    <t>0,0026563</t>
-  </si>
-  <si>
-    <t>0,0088543333333333333333333333</t>
-  </si>
-  <si>
-    <t>0,0177086666666666666666666667</t>
-  </si>
-  <si>
-    <t>0,026563</t>
+    <t>0,003</t>
+  </si>
+  <si>
+    <t>0,009</t>
+  </si>
+  <si>
+    <t>0,027</t>
   </si>
   <si>
     <t>32,85</t>
@@ -570,9 +564,6 @@
   </si>
   <si>
     <t>Устройство покрытий толщиной 15 см при укатке щебня с пределом прочности на сжатие свыше 68,6 до 98,1 МПа (свыше 700 до 1000 кгc/см2): однослойных</t>
-  </si>
-  <si>
-    <t>0,009</t>
   </si>
   <si>
     <t>45,18</t>
@@ -925,8 +916,8 @@
     <col min="1" max="1" width="52.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="178" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="138.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -952,24 +943,24 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C3">
-        <v>2</v>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C4">
+      <c r="B4">
         <v>70122</v>
       </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
       <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -991,24 +982,24 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>2</v>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7">
+      <c r="B7">
         <v>70122</v>
       </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
       <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1030,35 +1021,35 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>2</v>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10">
+      <c r="B10">
         <v>60259</v>
       </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
       <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C11">
+      <c r="B11">
         <v>70149</v>
       </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
       <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1114,24 +1105,24 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <v>2</v>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C16">
+      <c r="B16">
         <v>120202</v>
       </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
       <c r="D16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1153,35 +1144,35 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C18">
-        <v>2</v>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C19">
+      <c r="B19">
         <v>70149</v>
       </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
       <c r="D19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C20">
+      <c r="B20">
         <v>400051</v>
       </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
       <c r="D20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1203,46 +1194,46 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C22">
-        <v>2</v>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C23">
+      <c r="B23">
         <v>10312</v>
       </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
       <c r="D23" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C24">
+      <c r="B24">
         <v>70149</v>
       </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
       <c r="D24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C25">
+      <c r="B25">
         <v>120711</v>
       </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
       <c r="D25" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1264,35 +1255,35 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C27">
-        <v>2</v>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C28">
+      <c r="B28">
         <v>10312</v>
       </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
       <c r="D28" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C29">
+      <c r="B29">
         <v>120711</v>
       </c>
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
       <c r="D29" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1314,46 +1305,46 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C31">
-        <v>2</v>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C32">
+      <c r="B32">
         <v>60248</v>
       </c>
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
       <c r="D32" t="s">
-        <v>48</v>
-      </c>
-      <c r="E32" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C33">
+      <c r="B33">
         <v>70149</v>
       </c>
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
       <c r="D33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C34">
+      <c r="B34">
         <v>120202</v>
       </c>
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
       <c r="D34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1375,24 +1366,24 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C36">
-        <v>2</v>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C37">
+      <c r="B37">
         <v>70122</v>
       </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
       <c r="D37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1414,24 +1405,24 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C39">
-        <v>2</v>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>4</v>
-      </c>
-      <c r="E39" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C40">
+      <c r="B40">
         <v>70122</v>
       </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
       <c r="D40" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1453,35 +1444,35 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C42">
-        <v>2</v>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C43">
+      <c r="B43">
         <v>60259</v>
       </c>
+      <c r="C43" t="s">
+        <v>14</v>
+      </c>
       <c r="D43" t="s">
-        <v>14</v>
-      </c>
-      <c r="E43" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C44">
+      <c r="B44">
         <v>70149</v>
       </c>
+      <c r="C44" t="s">
+        <v>16</v>
+      </c>
       <c r="D44" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1537,24 +1528,24 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C48">
-        <v>2</v>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>4</v>
-      </c>
-      <c r="E48" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C49">
+      <c r="B49">
         <v>120202</v>
       </c>
+      <c r="C49" t="s">
+        <v>28</v>
+      </c>
       <c r="D49" t="s">
-        <v>28</v>
-      </c>
-      <c r="E49" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1576,35 +1567,35 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C51">
-        <v>2</v>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>4</v>
       </c>
       <c r="D51" t="s">
-        <v>4</v>
-      </c>
-      <c r="E51" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C52">
+      <c r="B52">
         <v>70149</v>
       </c>
+      <c r="C52" t="s">
+        <v>16</v>
+      </c>
       <c r="D52" t="s">
-        <v>16</v>
-      </c>
-      <c r="E52" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C53">
+      <c r="B53">
         <v>400051</v>
       </c>
+      <c r="C53" t="s">
+        <v>32</v>
+      </c>
       <c r="D53" t="s">
-        <v>32</v>
-      </c>
-      <c r="E53" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1622,50 +1613,50 @@
         <v>36</v>
       </c>
       <c r="E54" s="1">
-        <v>1.52871287128712E+28</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C55">
-        <v>2</v>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>4</v>
-      </c>
-      <c r="E55" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C56">
+      <c r="B56">
         <v>10312</v>
       </c>
+      <c r="C56" t="s">
+        <v>38</v>
+      </c>
       <c r="D56" t="s">
-        <v>38</v>
-      </c>
-      <c r="E56" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C57">
+      <c r="B57">
         <v>70149</v>
       </c>
+      <c r="C57" t="s">
+        <v>16</v>
+      </c>
       <c r="D57" t="s">
-        <v>16</v>
-      </c>
-      <c r="E57" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C58">
+      <c r="B58">
         <v>120711</v>
       </c>
+      <c r="C58" t="s">
+        <v>41</v>
+      </c>
       <c r="D58" t="s">
-        <v>41</v>
-      </c>
-      <c r="E58" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1683,39 +1674,39 @@
         <v>36</v>
       </c>
       <c r="E59" s="1">
-        <v>1.52871287128712E+28</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C60">
-        <v>2</v>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>4</v>
       </c>
       <c r="D60" t="s">
-        <v>4</v>
-      </c>
-      <c r="E60" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C61">
+      <c r="B61">
         <v>10312</v>
       </c>
+      <c r="C61" t="s">
+        <v>38</v>
+      </c>
       <c r="D61" t="s">
-        <v>38</v>
-      </c>
-      <c r="E61" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C62">
+      <c r="B62">
         <v>120711</v>
       </c>
+      <c r="C62" t="s">
+        <v>41</v>
+      </c>
       <c r="D62" t="s">
-        <v>41</v>
-      </c>
-      <c r="E62" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1737,46 +1728,46 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C64">
-        <v>2</v>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4</v>
       </c>
       <c r="D64" t="s">
-        <v>4</v>
-      </c>
-      <c r="E64" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C65">
+      <c r="B65">
         <v>60248</v>
       </c>
+      <c r="C65" t="s">
+        <v>48</v>
+      </c>
       <c r="D65" t="s">
-        <v>48</v>
-      </c>
-      <c r="E65" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C66">
+      <c r="B66">
         <v>70149</v>
       </c>
+      <c r="C66" t="s">
+        <v>16</v>
+      </c>
       <c r="D66" t="s">
-        <v>16</v>
-      </c>
-      <c r="E66" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C67">
+      <c r="B67">
         <v>120202</v>
       </c>
+      <c r="C67" t="s">
+        <v>28</v>
+      </c>
       <c r="D67" t="s">
-        <v>28</v>
-      </c>
-      <c r="E67" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1803,24 +1794,24 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C70">
-        <v>2</v>
+      <c r="B70">
+        <v>2</v>
+      </c>
+      <c r="C70" t="s">
+        <v>4</v>
       </c>
       <c r="D70" t="s">
-        <v>4</v>
-      </c>
-      <c r="E70" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C71">
+      <c r="B71">
         <v>60248</v>
       </c>
+      <c r="C71" t="s">
+        <v>48</v>
+      </c>
       <c r="D71" t="s">
-        <v>48</v>
-      </c>
-      <c r="E71" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1842,24 +1833,24 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C73">
-        <v>2</v>
-      </c>
-      <c r="D73" t="s">
-        <v>4</v>
-      </c>
-      <c r="E73">
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73">
         <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C74">
+      <c r="B74">
         <v>70150</v>
       </c>
-      <c r="D74" t="s">
+      <c r="C74" t="s">
         <v>66</v>
       </c>
-      <c r="E74">
+      <c r="D74">
         <v>11</v>
       </c>
     </row>
@@ -1881,46 +1872,46 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C76">
-        <v>2</v>
+      <c r="B76">
+        <v>2</v>
+      </c>
+      <c r="C76" t="s">
+        <v>4</v>
       </c>
       <c r="D76" t="s">
-        <v>4</v>
-      </c>
-      <c r="E76" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C77">
+      <c r="B77">
         <v>60248</v>
       </c>
+      <c r="C77" t="s">
+        <v>48</v>
+      </c>
       <c r="D77" t="s">
-        <v>48</v>
-      </c>
-      <c r="E77" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C78">
+      <c r="B78">
         <v>70149</v>
       </c>
+      <c r="C78" t="s">
+        <v>16</v>
+      </c>
       <c r="D78" t="s">
-        <v>16</v>
-      </c>
-      <c r="E78" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C79">
+      <c r="B79">
         <v>120202</v>
       </c>
-      <c r="D79" t="s">
+      <c r="C79" t="s">
         <v>28</v>
       </c>
-      <c r="E79">
+      <c r="D79">
         <v>1</v>
       </c>
     </row>
@@ -1942,35 +1933,35 @@
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C81">
-        <v>2</v>
+      <c r="B81">
+        <v>2</v>
+      </c>
+      <c r="C81" t="s">
+        <v>4</v>
       </c>
       <c r="D81" t="s">
-        <v>4</v>
-      </c>
-      <c r="E81" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C82">
+      <c r="B82">
         <v>120202</v>
       </c>
+      <c r="C82" t="s">
+        <v>28</v>
+      </c>
       <c r="D82" t="s">
-        <v>28</v>
-      </c>
-      <c r="E82" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C83">
+      <c r="B83">
         <v>400001</v>
       </c>
+      <c r="C83" t="s">
+        <v>77</v>
+      </c>
       <c r="D83" t="s">
-        <v>77</v>
-      </c>
-      <c r="E83" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2026,24 +2017,24 @@
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C87">
-        <v>2</v>
+      <c r="B87">
+        <v>2</v>
+      </c>
+      <c r="C87" t="s">
+        <v>4</v>
       </c>
       <c r="D87" t="s">
-        <v>4</v>
-      </c>
-      <c r="E87" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C88">
+      <c r="B88">
         <v>70150</v>
       </c>
+      <c r="C88" t="s">
+        <v>66</v>
+      </c>
       <c r="D88" t="s">
-        <v>66</v>
-      </c>
-      <c r="E88" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2065,24 +2056,24 @@
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C90">
-        <v>2</v>
+      <c r="B90">
+        <v>2</v>
+      </c>
+      <c r="C90" t="s">
+        <v>4</v>
       </c>
       <c r="D90" t="s">
-        <v>4</v>
-      </c>
-      <c r="E90" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C91">
+      <c r="B91">
         <v>70150</v>
       </c>
+      <c r="C91" t="s">
+        <v>66</v>
+      </c>
       <c r="D91" t="s">
-        <v>66</v>
-      </c>
-      <c r="E91" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2104,35 +2095,35 @@
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C93">
-        <v>2</v>
+      <c r="B93">
+        <v>2</v>
+      </c>
+      <c r="C93" t="s">
+        <v>4</v>
       </c>
       <c r="D93" t="s">
-        <v>4</v>
-      </c>
-      <c r="E93" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C94">
+      <c r="B94">
         <v>50102</v>
       </c>
+      <c r="C94" t="s">
+        <v>96</v>
+      </c>
       <c r="D94" t="s">
-        <v>96</v>
-      </c>
-      <c r="E94" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C95">
+      <c r="B95">
         <v>331100</v>
       </c>
+      <c r="C95" t="s">
+        <v>97</v>
+      </c>
       <c r="D95" t="s">
-        <v>97</v>
-      </c>
-      <c r="E95" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2154,24 +2145,24 @@
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C97">
-        <v>2</v>
+      <c r="B97">
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
+        <v>4</v>
       </c>
       <c r="D97" t="s">
-        <v>4</v>
-      </c>
-      <c r="E97" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C98">
+      <c r="B98">
         <v>70122</v>
       </c>
+      <c r="C98" t="s">
+        <v>6</v>
+      </c>
       <c r="D98" t="s">
-        <v>6</v>
-      </c>
-      <c r="E98" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2193,24 +2184,24 @@
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C100">
-        <v>2</v>
+      <c r="B100">
+        <v>2</v>
+      </c>
+      <c r="C100" t="s">
+        <v>4</v>
       </c>
       <c r="D100" t="s">
-        <v>4</v>
-      </c>
-      <c r="E100" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C101">
+      <c r="B101">
         <v>70122</v>
       </c>
+      <c r="C101" t="s">
+        <v>6</v>
+      </c>
       <c r="D101" t="s">
-        <v>6</v>
-      </c>
-      <c r="E101" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2232,35 +2223,35 @@
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C103">
-        <v>2</v>
+      <c r="B103">
+        <v>2</v>
+      </c>
+      <c r="C103" t="s">
+        <v>4</v>
       </c>
       <c r="D103" t="s">
-        <v>4</v>
-      </c>
-      <c r="E103" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C104">
+      <c r="B104">
         <v>60259</v>
       </c>
+      <c r="C104" t="s">
+        <v>14</v>
+      </c>
       <c r="D104" t="s">
-        <v>14</v>
-      </c>
-      <c r="E104" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C105">
+      <c r="B105">
         <v>70149</v>
       </c>
+      <c r="C105" t="s">
+        <v>16</v>
+      </c>
       <c r="D105" t="s">
-        <v>16</v>
-      </c>
-      <c r="E105" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2278,7 +2269,7 @@
         <v>20</v>
       </c>
       <c r="E106" s="1">
-        <v>6.07683333333333E+28</v>
+        <v>60768</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2295,7 +2286,7 @@
         <v>23</v>
       </c>
       <c r="E107" s="1">
-        <v>1.0634458333333301E+28</v>
+        <v>106345</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2316,24 +2307,24 @@
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C109">
-        <v>2</v>
+      <c r="B109">
+        <v>2</v>
+      </c>
+      <c r="C109" t="s">
+        <v>4</v>
       </c>
       <c r="D109" t="s">
-        <v>4</v>
-      </c>
-      <c r="E109" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C110">
+      <c r="B110">
         <v>120202</v>
       </c>
+      <c r="C110" t="s">
+        <v>28</v>
+      </c>
       <c r="D110" t="s">
-        <v>28</v>
-      </c>
-      <c r="E110" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2355,35 +2346,35 @@
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C112">
-        <v>2</v>
+      <c r="B112">
+        <v>2</v>
+      </c>
+      <c r="C112" t="s">
+        <v>4</v>
       </c>
       <c r="D112" t="s">
-        <v>4</v>
-      </c>
-      <c r="E112" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C113">
+      <c r="B113">
         <v>70149</v>
       </c>
+      <c r="C113" t="s">
+        <v>16</v>
+      </c>
       <c r="D113" t="s">
-        <v>16</v>
-      </c>
-      <c r="E113" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C114">
+      <c r="B114">
         <v>400051</v>
       </c>
+      <c r="C114" t="s">
+        <v>32</v>
+      </c>
       <c r="D114" t="s">
-        <v>32</v>
-      </c>
-      <c r="E114" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2405,24 +2396,24 @@
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C116">
-        <v>2</v>
+      <c r="B116">
+        <v>2</v>
+      </c>
+      <c r="C116" t="s">
+        <v>4</v>
       </c>
       <c r="D116" t="s">
-        <v>4</v>
-      </c>
-      <c r="E116" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C117">
+      <c r="B117">
         <v>70122</v>
       </c>
+      <c r="C117" t="s">
+        <v>6</v>
+      </c>
       <c r="D117" t="s">
-        <v>6</v>
-      </c>
-      <c r="E117" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2444,24 +2435,24 @@
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C119">
-        <v>2</v>
+      <c r="B119">
+        <v>2</v>
+      </c>
+      <c r="C119" t="s">
+        <v>4</v>
       </c>
       <c r="D119" t="s">
-        <v>4</v>
-      </c>
-      <c r="E119" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C120">
+      <c r="B120">
         <v>70122</v>
       </c>
+      <c r="C120" t="s">
+        <v>6</v>
+      </c>
       <c r="D120" t="s">
-        <v>6</v>
-      </c>
-      <c r="E120" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2500,24 +2491,24 @@
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C123">
-        <v>2</v>
+      <c r="B123">
+        <v>2</v>
+      </c>
+      <c r="C123" t="s">
+        <v>4</v>
       </c>
       <c r="D123" t="s">
-        <v>4</v>
-      </c>
-      <c r="E123" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C124">
+      <c r="B124">
         <v>70223</v>
       </c>
+      <c r="C124" t="s">
+        <v>114</v>
+      </c>
       <c r="D124" t="s">
-        <v>114</v>
-      </c>
-      <c r="E124" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2539,24 +2530,24 @@
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C126">
-        <v>2</v>
+      <c r="B126">
+        <v>2</v>
+      </c>
+      <c r="C126" t="s">
+        <v>4</v>
       </c>
       <c r="D126" t="s">
-        <v>4</v>
-      </c>
-      <c r="E126" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C127">
+      <c r="B127">
         <v>70150</v>
       </c>
+      <c r="C127" t="s">
+        <v>66</v>
+      </c>
       <c r="D127" t="s">
-        <v>66</v>
-      </c>
-      <c r="E127" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2578,24 +2569,24 @@
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C129">
-        <v>2</v>
+      <c r="B129">
+        <v>2</v>
+      </c>
+      <c r="C129" t="s">
+        <v>4</v>
       </c>
       <c r="D129" t="s">
-        <v>4</v>
-      </c>
-      <c r="E129" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C130">
+      <c r="B130">
         <v>70150</v>
       </c>
+      <c r="C130" t="s">
+        <v>66</v>
+      </c>
       <c r="D130" t="s">
-        <v>66</v>
-      </c>
-      <c r="E130" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2617,35 +2608,35 @@
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C132">
-        <v>2</v>
+      <c r="B132">
+        <v>2</v>
+      </c>
+      <c r="C132" t="s">
+        <v>4</v>
       </c>
       <c r="D132" t="s">
-        <v>4</v>
-      </c>
-      <c r="E132" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C133">
+      <c r="B133">
         <v>60259</v>
       </c>
+      <c r="C133" t="s">
+        <v>14</v>
+      </c>
       <c r="D133" t="s">
-        <v>14</v>
-      </c>
-      <c r="E133" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C134">
+      <c r="B134">
         <v>70149</v>
       </c>
+      <c r="C134" t="s">
+        <v>16</v>
+      </c>
       <c r="D134" t="s">
-        <v>16</v>
-      </c>
-      <c r="E134" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2684,24 +2675,24 @@
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C137">
-        <v>2</v>
+      <c r="B137">
+        <v>2</v>
+      </c>
+      <c r="C137" t="s">
+        <v>4</v>
       </c>
       <c r="D137" t="s">
-        <v>4</v>
-      </c>
-      <c r="E137" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C138">
+      <c r="B138">
         <v>120202</v>
       </c>
+      <c r="C138" t="s">
+        <v>28</v>
+      </c>
       <c r="D138" t="s">
-        <v>28</v>
-      </c>
-      <c r="E138" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2723,35 +2714,35 @@
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C140">
-        <v>2</v>
+      <c r="B140">
+        <v>2</v>
+      </c>
+      <c r="C140" t="s">
+        <v>4</v>
       </c>
       <c r="D140" t="s">
-        <v>4</v>
-      </c>
-      <c r="E140" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C141">
+      <c r="B141">
         <v>70149</v>
       </c>
+      <c r="C141" t="s">
+        <v>16</v>
+      </c>
       <c r="D141" t="s">
-        <v>16</v>
-      </c>
-      <c r="E141" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C142">
+      <c r="B142">
         <v>400051</v>
       </c>
+      <c r="C142" t="s">
+        <v>32</v>
+      </c>
       <c r="D142" t="s">
-        <v>32</v>
-      </c>
-      <c r="E142" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2773,46 +2764,46 @@
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C144">
-        <v>2</v>
+      <c r="B144">
+        <v>2</v>
+      </c>
+      <c r="C144" t="s">
+        <v>4</v>
       </c>
       <c r="D144" t="s">
-        <v>4</v>
-      </c>
-      <c r="E144" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C145">
+      <c r="B145">
         <v>60248</v>
       </c>
+      <c r="C145" t="s">
+        <v>48</v>
+      </c>
       <c r="D145" t="s">
-        <v>48</v>
-      </c>
-      <c r="E145" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C146">
+      <c r="B146">
         <v>70148</v>
       </c>
+      <c r="C146" t="s">
+        <v>131</v>
+      </c>
       <c r="D146" t="s">
-        <v>131</v>
-      </c>
-      <c r="E146" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C147">
+      <c r="B147">
         <v>130300</v>
       </c>
+      <c r="C147" t="s">
+        <v>132</v>
+      </c>
       <c r="D147" t="s">
-        <v>132</v>
-      </c>
-      <c r="E147" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2856,24 +2847,24 @@
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C151">
-        <v>2</v>
+      <c r="B151">
+        <v>2</v>
+      </c>
+      <c r="C151" t="s">
+        <v>4</v>
       </c>
       <c r="D151" t="s">
-        <v>4</v>
-      </c>
-      <c r="E151" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C152">
+      <c r="B152">
         <v>70122</v>
       </c>
+      <c r="C152" t="s">
+        <v>6</v>
+      </c>
       <c r="D152" t="s">
-        <v>6</v>
-      </c>
-      <c r="E152" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2895,24 +2886,24 @@
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C154">
-        <v>2</v>
+      <c r="B154">
+        <v>2</v>
+      </c>
+      <c r="C154" t="s">
+        <v>4</v>
       </c>
       <c r="D154" t="s">
-        <v>4</v>
-      </c>
-      <c r="E154" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C155">
+      <c r="B155">
         <v>70122</v>
       </c>
+      <c r="C155" t="s">
+        <v>6</v>
+      </c>
       <c r="D155" t="s">
-        <v>6</v>
-      </c>
-      <c r="E155" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2934,35 +2925,35 @@
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C157">
-        <v>2</v>
+      <c r="B157">
+        <v>2</v>
+      </c>
+      <c r="C157" t="s">
+        <v>4</v>
       </c>
       <c r="D157" t="s">
-        <v>4</v>
-      </c>
-      <c r="E157" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C158">
+      <c r="B158">
         <v>60259</v>
       </c>
+      <c r="C158" t="s">
+        <v>14</v>
+      </c>
       <c r="D158" t="s">
-        <v>14</v>
-      </c>
-      <c r="E158" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C159">
+      <c r="B159">
         <v>70149</v>
       </c>
+      <c r="C159" t="s">
+        <v>16</v>
+      </c>
       <c r="D159" t="s">
-        <v>16</v>
-      </c>
-      <c r="E159" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3018,24 +3009,24 @@
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C163">
-        <v>2</v>
+      <c r="B163">
+        <v>2</v>
+      </c>
+      <c r="C163" t="s">
+        <v>4</v>
       </c>
       <c r="D163" t="s">
-        <v>4</v>
-      </c>
-      <c r="E163" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C164">
+      <c r="B164">
         <v>120202</v>
       </c>
+      <c r="C164" t="s">
+        <v>28</v>
+      </c>
       <c r="D164" t="s">
-        <v>28</v>
-      </c>
-      <c r="E164" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3057,35 +3048,35 @@
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C166">
-        <v>2</v>
+      <c r="B166">
+        <v>2</v>
+      </c>
+      <c r="C166" t="s">
+        <v>4</v>
       </c>
       <c r="D166" t="s">
-        <v>4</v>
-      </c>
-      <c r="E166" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C167">
+      <c r="B167">
         <v>70149</v>
       </c>
+      <c r="C167" t="s">
+        <v>16</v>
+      </c>
       <c r="D167" t="s">
-        <v>16</v>
-      </c>
-      <c r="E167" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C168">
+      <c r="B168">
         <v>400051</v>
       </c>
+      <c r="C168" t="s">
+        <v>32</v>
+      </c>
       <c r="D168" t="s">
-        <v>32</v>
-      </c>
-      <c r="E168" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3107,46 +3098,46 @@
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C170">
-        <v>2</v>
+      <c r="B170">
+        <v>2</v>
+      </c>
+      <c r="C170" t="s">
+        <v>4</v>
       </c>
       <c r="D170" t="s">
-        <v>4</v>
-      </c>
-      <c r="E170" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C171">
+      <c r="B171">
         <v>60248</v>
       </c>
+      <c r="C171" t="s">
+        <v>48</v>
+      </c>
       <c r="D171" t="s">
-        <v>48</v>
-      </c>
-      <c r="E171" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C172">
+      <c r="B172">
         <v>70149</v>
       </c>
+      <c r="C172" t="s">
+        <v>16</v>
+      </c>
       <c r="D172" t="s">
-        <v>16</v>
-      </c>
-      <c r="E172" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C173">
+      <c r="B173">
         <v>120202</v>
       </c>
+      <c r="C173" t="s">
+        <v>28</v>
+      </c>
       <c r="D173" t="s">
-        <v>28</v>
-      </c>
-      <c r="E173" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3168,13 +3159,13 @@
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C175">
+      <c r="B175">
         <v>400001</v>
       </c>
+      <c r="C175" t="s">
+        <v>77</v>
+      </c>
       <c r="D175" t="s">
-        <v>77</v>
-      </c>
-      <c r="E175" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3209,7 +3200,7 @@
         <v>84</v>
       </c>
       <c r="E177" t="s">
-        <v>146</v>
+        <v>62</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -3226,28 +3217,28 @@
         <v>3</v>
       </c>
       <c r="E178" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C179">
-        <v>2</v>
+      <c r="B179">
+        <v>2</v>
+      </c>
+      <c r="C179" t="s">
+        <v>4</v>
       </c>
       <c r="D179" t="s">
-        <v>4</v>
-      </c>
-      <c r="E179" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C180">
+      <c r="B180">
         <v>70122</v>
       </c>
+      <c r="C180" t="s">
+        <v>6</v>
+      </c>
       <c r="D180" t="s">
-        <v>6</v>
-      </c>
-      <c r="E180" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3265,28 +3256,28 @@
         <v>3</v>
       </c>
       <c r="E181" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C182">
-        <v>2</v>
+      <c r="B182">
+        <v>2</v>
+      </c>
+      <c r="C182" t="s">
+        <v>4</v>
       </c>
       <c r="D182" t="s">
-        <v>4</v>
-      </c>
-      <c r="E182" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C183">
+      <c r="B183">
         <v>70122</v>
       </c>
+      <c r="C183" t="s">
+        <v>6</v>
+      </c>
       <c r="D183" t="s">
-        <v>6</v>
-      </c>
-      <c r="E183" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3304,39 +3295,39 @@
         <v>3</v>
       </c>
       <c r="E184" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C185">
-        <v>2</v>
+      <c r="B185">
+        <v>2</v>
+      </c>
+      <c r="C185" t="s">
+        <v>4</v>
       </c>
       <c r="D185" t="s">
-        <v>4</v>
-      </c>
-      <c r="E185" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C186">
+      <c r="B186">
         <v>60259</v>
       </c>
+      <c r="C186" t="s">
+        <v>14</v>
+      </c>
       <c r="D186" t="s">
-        <v>14</v>
-      </c>
-      <c r="E186" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C187">
+      <c r="B187">
         <v>70149</v>
       </c>
+      <c r="C187" t="s">
+        <v>16</v>
+      </c>
       <c r="D187" t="s">
-        <v>16</v>
-      </c>
-      <c r="E187" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3354,7 +3345,7 @@
         <v>20</v>
       </c>
       <c r="E188" s="1">
-        <v>8.8543333333333305E+27</v>
+        <v>8854</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -3371,7 +3362,7 @@
         <v>23</v>
       </c>
       <c r="E189" s="1">
-        <v>1.5495083333333299E+28</v>
+        <v>15495</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -3388,28 +3379,28 @@
         <v>3</v>
       </c>
       <c r="E190" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C191">
-        <v>2</v>
+      <c r="B191">
+        <v>2</v>
+      </c>
+      <c r="C191" t="s">
+        <v>4</v>
       </c>
       <c r="D191" t="s">
-        <v>4</v>
-      </c>
-      <c r="E191" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C192">
+      <c r="B192">
         <v>120202</v>
       </c>
+      <c r="C192" t="s">
+        <v>28</v>
+      </c>
       <c r="D192" t="s">
-        <v>28</v>
-      </c>
-      <c r="E192" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3427,39 +3418,39 @@
         <v>3</v>
       </c>
       <c r="E193" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C194">
-        <v>2</v>
+      <c r="B194">
+        <v>2</v>
+      </c>
+      <c r="C194" t="s">
+        <v>4</v>
       </c>
       <c r="D194" t="s">
-        <v>4</v>
-      </c>
-      <c r="E194" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C195">
+      <c r="B195">
         <v>70149</v>
       </c>
+      <c r="C195" t="s">
+        <v>16</v>
+      </c>
       <c r="D195" t="s">
-        <v>16</v>
-      </c>
-      <c r="E195" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C196">
+      <c r="B196">
         <v>400051</v>
       </c>
+      <c r="C196" t="s">
+        <v>32</v>
+      </c>
       <c r="D196" t="s">
-        <v>32</v>
-      </c>
-      <c r="E196" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3477,28 +3468,28 @@
         <v>3</v>
       </c>
       <c r="E197" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C198">
-        <v>2</v>
+      <c r="B198">
+        <v>2</v>
+      </c>
+      <c r="C198" t="s">
+        <v>4</v>
       </c>
       <c r="D198" t="s">
-        <v>4</v>
-      </c>
-      <c r="E198" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C199">
+      <c r="B199">
         <v>70122</v>
       </c>
+      <c r="C199" t="s">
+        <v>6</v>
+      </c>
       <c r="D199" t="s">
-        <v>6</v>
-      </c>
-      <c r="E199" t="s">
         <v>106</v>
       </c>
     </row>
@@ -3516,28 +3507,28 @@
         <v>3</v>
       </c>
       <c r="E200" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C201">
-        <v>2</v>
+      <c r="B201">
+        <v>2</v>
+      </c>
+      <c r="C201" t="s">
+        <v>4</v>
       </c>
       <c r="D201" t="s">
-        <v>4</v>
-      </c>
-      <c r="E201" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C202">
+      <c r="B202">
         <v>70122</v>
       </c>
+      <c r="C202" t="s">
+        <v>6</v>
+      </c>
       <c r="D202" t="s">
-        <v>6</v>
-      </c>
-      <c r="E202" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3555,7 +3546,7 @@
         <v>20</v>
       </c>
       <c r="E203" s="1">
-        <v>1.7708666666666599E+28</v>
+        <v>17709</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -3572,28 +3563,28 @@
         <v>3</v>
       </c>
       <c r="E204" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C205">
-        <v>2</v>
+      <c r="B205">
+        <v>2</v>
+      </c>
+      <c r="C205" t="s">
+        <v>4</v>
       </c>
       <c r="D205" t="s">
-        <v>4</v>
-      </c>
-      <c r="E205" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C206">
+      <c r="B206">
         <v>70223</v>
       </c>
+      <c r="C206" t="s">
+        <v>114</v>
+      </c>
       <c r="D206" t="s">
-        <v>114</v>
-      </c>
-      <c r="E206" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3611,28 +3602,28 @@
         <v>3</v>
       </c>
       <c r="E207" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C208">
-        <v>2</v>
+      <c r="B208">
+        <v>2</v>
+      </c>
+      <c r="C208" t="s">
+        <v>4</v>
       </c>
       <c r="D208" t="s">
-        <v>4</v>
-      </c>
-      <c r="E208" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C209">
+      <c r="B209">
         <v>70150</v>
       </c>
+      <c r="C209" t="s">
+        <v>66</v>
+      </c>
       <c r="D209" t="s">
-        <v>66</v>
-      </c>
-      <c r="E209" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3650,28 +3641,28 @@
         <v>3</v>
       </c>
       <c r="E210" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C211">
-        <v>2</v>
+      <c r="B211">
+        <v>2</v>
+      </c>
+      <c r="C211" t="s">
+        <v>4</v>
       </c>
       <c r="D211" t="s">
-        <v>4</v>
-      </c>
-      <c r="E211" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C212">
+      <c r="B212">
         <v>70150</v>
       </c>
+      <c r="C212" t="s">
+        <v>66</v>
+      </c>
       <c r="D212" t="s">
-        <v>66</v>
-      </c>
-      <c r="E212" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3689,39 +3680,39 @@
         <v>3</v>
       </c>
       <c r="E213" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C214">
-        <v>2</v>
+      <c r="B214">
+        <v>2</v>
+      </c>
+      <c r="C214" t="s">
+        <v>4</v>
       </c>
       <c r="D214" t="s">
-        <v>4</v>
-      </c>
-      <c r="E214" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C215">
+      <c r="B215">
         <v>60259</v>
       </c>
+      <c r="C215" t="s">
+        <v>14</v>
+      </c>
       <c r="D215" t="s">
-        <v>14</v>
-      </c>
-      <c r="E215" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C216">
+      <c r="B216">
         <v>70149</v>
       </c>
+      <c r="C216" t="s">
+        <v>16</v>
+      </c>
       <c r="D216" t="s">
-        <v>16</v>
-      </c>
-      <c r="E216" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3739,7 +3730,7 @@
         <v>23</v>
       </c>
       <c r="E217" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -3756,28 +3747,28 @@
         <v>3</v>
       </c>
       <c r="E218" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C219">
-        <v>2</v>
+      <c r="B219">
+        <v>2</v>
+      </c>
+      <c r="C219" t="s">
+        <v>4</v>
       </c>
       <c r="D219" t="s">
-        <v>4</v>
-      </c>
-      <c r="E219" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C220">
+      <c r="B220">
         <v>120202</v>
       </c>
+      <c r="C220" t="s">
+        <v>28</v>
+      </c>
       <c r="D220" t="s">
-        <v>28</v>
-      </c>
-      <c r="E220" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3795,39 +3786,39 @@
         <v>3</v>
       </c>
       <c r="E221" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C222">
-        <v>2</v>
+      <c r="B222">
+        <v>2</v>
+      </c>
+      <c r="C222" t="s">
+        <v>4</v>
       </c>
       <c r="D222" t="s">
-        <v>4</v>
-      </c>
-      <c r="E222" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C223">
+      <c r="B223">
         <v>70149</v>
       </c>
+      <c r="C223" t="s">
+        <v>16</v>
+      </c>
       <c r="D223" t="s">
-        <v>16</v>
-      </c>
-      <c r="E223" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C224">
+      <c r="B224">
         <v>400051</v>
       </c>
+      <c r="C224" t="s">
+        <v>32</v>
+      </c>
       <c r="D224" t="s">
-        <v>32</v>
-      </c>
-      <c r="E224" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3845,50 +3836,50 @@
         <v>127</v>
       </c>
       <c r="E225" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C226">
-        <v>2</v>
+      <c r="B226">
+        <v>2</v>
+      </c>
+      <c r="C226" t="s">
+        <v>4</v>
       </c>
       <c r="D226" t="s">
-        <v>4</v>
-      </c>
-      <c r="E226" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C227">
+      <c r="B227">
         <v>60248</v>
       </c>
+      <c r="C227" t="s">
+        <v>48</v>
+      </c>
       <c r="D227" t="s">
-        <v>48</v>
-      </c>
-      <c r="E227" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C228">
+      <c r="B228">
         <v>70148</v>
       </c>
+      <c r="C228" t="s">
+        <v>131</v>
+      </c>
       <c r="D228" t="s">
-        <v>131</v>
-      </c>
-      <c r="E228" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C229">
+      <c r="B229">
         <v>130300</v>
       </c>
+      <c r="C229" t="s">
+        <v>132</v>
+      </c>
       <c r="D229" t="s">
-        <v>132</v>
-      </c>
-      <c r="E229" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3911,7 +3902,7 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -3919,93 +3910,93 @@
         <v>1</v>
       </c>
       <c r="B232" t="s">
+        <v>152</v>
+      </c>
+      <c r="C232" t="s">
+        <v>153</v>
+      </c>
+      <c r="D232" t="s">
         <v>154</v>
       </c>
-      <c r="C232" t="s">
+      <c r="E232" t="s">
         <v>155</v>
       </c>
-      <c r="D232" t="s">
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B233">
+        <v>2</v>
+      </c>
+      <c r="C233" t="s">
+        <v>4</v>
+      </c>
+      <c r="D233" t="s">
         <v>156</v>
       </c>
-      <c r="E232" t="s">
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B234">
+        <v>30101</v>
+      </c>
+      <c r="C234" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C233">
-        <v>2</v>
-      </c>
-      <c r="D233" t="s">
-        <v>4</v>
-      </c>
-      <c r="E233" t="s">
+      <c r="D234" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C234">
-        <v>30101</v>
-      </c>
-      <c r="D234" t="s">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B235">
+        <v>70149</v>
+      </c>
+      <c r="C235" t="s">
+        <v>16</v>
+      </c>
+      <c r="D235" t="s">
         <v>159</v>
       </c>
-      <c r="E234" t="s">
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B236">
+        <v>120202</v>
+      </c>
+      <c r="C236" t="s">
+        <v>28</v>
+      </c>
+      <c r="D236" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C235">
-        <v>70149</v>
-      </c>
-      <c r="D235" t="s">
-        <v>16</v>
-      </c>
-      <c r="E235" t="s">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B237">
+        <v>120906</v>
+      </c>
+      <c r="C237" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C236">
-        <v>120202</v>
-      </c>
-      <c r="D236" t="s">
-        <v>28</v>
-      </c>
-      <c r="E236" t="s">
+      <c r="D237" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C237">
-        <v>120906</v>
-      </c>
-      <c r="D237" t="s">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B238">
+        <v>120907</v>
+      </c>
+      <c r="C238" t="s">
         <v>163</v>
       </c>
-      <c r="E237" t="s">
+      <c r="D238" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C238">
-        <v>120907</v>
-      </c>
-      <c r="D238" t="s">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B239">
+        <v>121601</v>
+      </c>
+      <c r="C239" t="s">
         <v>165</v>
       </c>
-      <c r="E238" t="s">
+      <c r="D239" t="s">
         <v>166</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C239">
-        <v>121601</v>
-      </c>
-      <c r="D239" t="s">
-        <v>167</v>
-      </c>
-      <c r="E239" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
@@ -4013,93 +4004,93 @@
         <v>2</v>
       </c>
       <c r="B240" t="s">
+        <v>167</v>
+      </c>
+      <c r="C240" t="s">
+        <v>168</v>
+      </c>
+      <c r="D240" t="s">
+        <v>154</v>
+      </c>
+      <c r="E240" t="s">
         <v>169</v>
       </c>
-      <c r="C240" t="s">
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B241">
+        <v>2</v>
+      </c>
+      <c r="C241" t="s">
+        <v>4</v>
+      </c>
+      <c r="D241" t="s">
         <v>170</v>
       </c>
-      <c r="D240" t="s">
-        <v>156</v>
-      </c>
-      <c r="E240" t="s">
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B242">
+        <v>30101</v>
+      </c>
+      <c r="C242" t="s">
+        <v>157</v>
+      </c>
+      <c r="D242" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C241">
-        <v>2</v>
-      </c>
-      <c r="D241" t="s">
-        <v>4</v>
-      </c>
-      <c r="E241" t="s">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B243">
+        <v>120202</v>
+      </c>
+      <c r="C243" t="s">
+        <v>28</v>
+      </c>
+      <c r="D243" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C242">
-        <v>30101</v>
-      </c>
-      <c r="D242" t="s">
-        <v>159</v>
-      </c>
-      <c r="E242" t="s">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B244">
+        <v>120906</v>
+      </c>
+      <c r="C244" t="s">
+        <v>161</v>
+      </c>
+      <c r="D244" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C243">
-        <v>120202</v>
-      </c>
-      <c r="D243" t="s">
-        <v>28</v>
-      </c>
-      <c r="E243" t="s">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B245">
+        <v>120907</v>
+      </c>
+      <c r="C245" t="s">
+        <v>163</v>
+      </c>
+      <c r="D245" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C244">
-        <v>120906</v>
-      </c>
-      <c r="D244" t="s">
-        <v>163</v>
-      </c>
-      <c r="E244" t="s">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B246">
+        <v>121601</v>
+      </c>
+      <c r="C246" t="s">
+        <v>165</v>
+      </c>
+      <c r="D246" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C245">
-        <v>120907</v>
-      </c>
-      <c r="D245" t="s">
-        <v>165</v>
-      </c>
-      <c r="E245" t="s">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B247">
+        <v>121803</v>
+      </c>
+      <c r="C247" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C246">
-        <v>121601</v>
-      </c>
-      <c r="D246" t="s">
-        <v>167</v>
-      </c>
-      <c r="E246" t="s">
+      <c r="D247" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C247">
-        <v>121803</v>
-      </c>
-      <c r="D247" t="s">
-        <v>178</v>
-      </c>
-      <c r="E247" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
@@ -4107,104 +4098,104 @@
         <v>3</v>
       </c>
       <c r="B248" t="s">
+        <v>178</v>
+      </c>
+      <c r="C248" t="s">
+        <v>179</v>
+      </c>
+      <c r="D248" t="s">
+        <v>154</v>
+      </c>
+      <c r="E248" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B249">
+        <v>2</v>
+      </c>
+      <c r="C249" t="s">
+        <v>4</v>
+      </c>
+      <c r="D249" t="s">
         <v>180</v>
       </c>
-      <c r="C248" t="s">
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B250">
+        <v>30101</v>
+      </c>
+      <c r="C250" t="s">
+        <v>157</v>
+      </c>
+      <c r="D250" t="s">
         <v>181</v>
       </c>
-      <c r="D248" t="s">
-        <v>156</v>
-      </c>
-      <c r="E248" t="s">
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B251">
+        <v>70149</v>
+      </c>
+      <c r="C251" t="s">
+        <v>16</v>
+      </c>
+      <c r="D251" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B252">
+        <v>120202</v>
+      </c>
+      <c r="C252" t="s">
+        <v>28</v>
+      </c>
+      <c r="D252" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B253">
+        <v>120906</v>
+      </c>
+      <c r="C253" t="s">
+        <v>161</v>
+      </c>
+      <c r="D253" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B254">
+        <v>120907</v>
+      </c>
+      <c r="C254" t="s">
+        <v>163</v>
+      </c>
+      <c r="D254" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C249">
-        <v>2</v>
-      </c>
-      <c r="D249" t="s">
-        <v>4</v>
-      </c>
-      <c r="E249" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C250">
-        <v>30101</v>
-      </c>
-      <c r="D250" t="s">
-        <v>159</v>
-      </c>
-      <c r="E250" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C251">
-        <v>70149</v>
-      </c>
-      <c r="D251" t="s">
-        <v>16</v>
-      </c>
-      <c r="E251" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C252">
-        <v>120202</v>
-      </c>
-      <c r="D252" t="s">
-        <v>28</v>
-      </c>
-      <c r="E252" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C253">
-        <v>120906</v>
-      </c>
-      <c r="D253" t="s">
-        <v>163</v>
-      </c>
-      <c r="E253" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C254">
-        <v>120907</v>
-      </c>
-      <c r="D254" t="s">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B255">
+        <v>121601</v>
+      </c>
+      <c r="C255" t="s">
         <v>165</v>
       </c>
-      <c r="E254" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C255">
-        <v>121601</v>
-      </c>
       <c r="D255" t="s">
-        <v>167</v>
-      </c>
-      <c r="E255" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C256">
+      <c r="B256">
         <v>121803</v>
       </c>
+      <c r="C256" t="s">
+        <v>176</v>
+      </c>
       <c r="D256" t="s">
-        <v>178</v>
-      </c>
-      <c r="E256" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
@@ -4212,60 +4203,60 @@
         <v>4</v>
       </c>
       <c r="B257" t="s">
+        <v>183</v>
+      </c>
+      <c r="C257" t="s">
+        <v>184</v>
+      </c>
+      <c r="D257" t="s">
+        <v>154</v>
+      </c>
+      <c r="E257" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B258">
+        <v>2</v>
+      </c>
+      <c r="C258" t="s">
+        <v>4</v>
+      </c>
+      <c r="D258" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B259">
+        <v>30101</v>
+      </c>
+      <c r="C259" t="s">
+        <v>157</v>
+      </c>
+      <c r="D259" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B260">
+        <v>120906</v>
+      </c>
+      <c r="C260" t="s">
+        <v>161</v>
+      </c>
+      <c r="D260" t="s">
         <v>186</v>
       </c>
-      <c r="C257" t="s">
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B261">
+        <v>120907</v>
+      </c>
+      <c r="C261" t="s">
+        <v>163</v>
+      </c>
+      <c r="D261" t="s">
         <v>187</v>
-      </c>
-      <c r="D257" t="s">
-        <v>156</v>
-      </c>
-      <c r="E257" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C258">
-        <v>2</v>
-      </c>
-      <c r="D258" t="s">
-        <v>4</v>
-      </c>
-      <c r="E258" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C259">
-        <v>30101</v>
-      </c>
-      <c r="D259" t="s">
-        <v>159</v>
-      </c>
-      <c r="E259" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C260">
-        <v>120906</v>
-      </c>
-      <c r="D260" t="s">
-        <v>163</v>
-      </c>
-      <c r="E260" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C261">
-        <v>120907</v>
-      </c>
-      <c r="D261" t="s">
-        <v>165</v>
-      </c>
-      <c r="E261" t="s">
-        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>